<commit_message>
multiple fixes, got html and pdf working again, but need to fix wrap
</commit_message>
<xml_diff>
--- a/data_out/updated_table_1.xlsx
+++ b/data_out/updated_table_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/paulukonis_elizabeth_epa_gov/Documents/Profile/Documents/GitHub/amphib_dermal_collation/data_out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{4A4EFD78-0907-4FC8-92B0-0B1CEC1C87FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFF44D08-3EBF-4FEC-BF7B-B40DD1884675}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{4A4EFD78-0907-4FC8-92B0-0B1CEC1C87FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5589C366-A86B-48D0-88C0-E5F4B28223DC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{270C0B6F-07D5-4ABF-8C8D-C27E7F4C0DCE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
   <si>
     <t>Study </t>
   </si>
@@ -377,11 +377,35 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t xml:space="preserve"> 0.322, 0.510, 0.390 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.130, 0.214, 0.177 </t>
+  </si>
+  <si>
+    <t>0.049, 0.148, 0.090</t>
+  </si>
+  <si>
+    <t>0.047, 0.275, 0.207</t>
+  </si>
+  <si>
+    <t>0.019, 0.108, 0.049</t>
+  </si>
+  <si>
+    <t>0.023, 0.068, 0.051</t>
+  </si>
+  <si>
+    <t>0.121, 0.192, 0.151</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -453,20 +477,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,21 +809,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3806413E-9CE4-4194-B643-88BCE59D4128}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.7265625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
-    <col min="3" max="3" width="15.90625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="6" customWidth="1"/>
     <col min="4" max="5" width="19.6328125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.1796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.6328125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="3"/>
+    <col min="8" max="9" width="8.7265625" style="6"/>
+    <col min="10" max="10" width="13.08984375" style="6" customWidth="1"/>
+    <col min="11" max="13" width="8.7265625" style="6"/>
+    <col min="14" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.35">
@@ -805,7 +836,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -828,7 +859,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -845,13 +876,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="7">
         <v>106</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -860,17 +891,17 @@
       <c r="E3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -880,11 +911,14 @@
         <v>74</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>63</v>
       </c>
@@ -892,12 +926,14 @@
         <v>75</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>64</v>
       </c>
@@ -905,12 +941,12 @@
         <v>76</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -920,12 +956,12 @@
         <v>77</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -935,12 +971,14 @@
         <v>78</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>67</v>
       </c>
@@ -948,12 +986,12 @@
         <v>79</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
         <v>59</v>
       </c>
@@ -963,12 +1001,12 @@
       <c r="F10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>62</v>
       </c>
@@ -976,12 +1014,12 @@
         <v>74</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
         <v>63</v>
       </c>
@@ -989,12 +1027,12 @@
         <v>75</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
         <v>64</v>
       </c>
@@ -1002,12 +1040,12 @@
         <v>76</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1015,12 +1053,12 @@
         <v>77</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1028,12 +1066,12 @@
         <v>78</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
@@ -1041,12 +1079,12 @@
         <v>79</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="2"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1056,12 +1094,12 @@
       <c r="F17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="2"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
         <v>62</v>
       </c>
@@ -1069,12 +1107,12 @@
         <v>74</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="2"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
         <v>63</v>
       </c>
@@ -1082,12 +1120,12 @@
         <v>75</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="2"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1095,12 +1133,12 @@
         <v>76</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="2"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
@@ -1108,12 +1146,12 @@
         <v>77</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1121,12 +1159,12 @@
         <v>78</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="2"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
         <v>67</v>
       </c>
@@ -1134,200 +1172,234 @@
         <v>79</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="2"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="2"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="2"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="2"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="2"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="2"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="2"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="2"/>
+      <c r="G31" s="8"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="2"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="8"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="2"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="8"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="2"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="8"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="2"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="8"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="2"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="8"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" ht="69" x14ac:dyDescent="0.35">
+      <c r="F37" s="10"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:13" ht="69" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1341,23 +1413,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="C39" s="4"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -1371,14 +1443,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1392,14 +1464,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1413,14 +1485,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1434,14 +1506,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1455,14 +1527,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1476,65 +1548,65 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="6"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="11"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-    </row>
-    <row r="48" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E48" s="1"/>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="6"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
@@ -1543,7 +1615,7 @@
       <c r="B50" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1558,7 +1630,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="F24:F30"/>
     <mergeCell ref="G3:G37"/>
     <mergeCell ref="B3:B37"/>
     <mergeCell ref="F3:F9"/>
@@ -1574,6 +1648,7 @@
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A3:A37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated all final rmd stuff, and added in script
</commit_message>
<xml_diff>
--- a/data_out/updated_table_1.xlsx
+++ b/data_out/updated_table_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/paulukonis_elizabeth_epa_gov/Documents/Profile/Documents/GitHub/amphib_dermal_collation/data_out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="8_{4A4EFD78-0907-4FC8-92B0-0B1CEC1C87FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37FEC539-2623-486A-963A-01E1F33D61C4}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="8_{4A4EFD78-0907-4FC8-92B0-0B1CEC1C87FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71203AA4-B89E-4978-B864-07E88C25E08E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{270C0B6F-07D5-4ABF-8C8D-C27E7F4C0DCE}"/>
   </bookViews>
@@ -471,9 +471,6 @@
     <t>0.02, 0.417, 0.141</t>
   </si>
   <si>
-    <t>Glinski et al. 2020</t>
-  </si>
-  <si>
     <t>0.227, 0.613, 0.328</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   </si>
   <si>
     <t>0, 1.909, 0.417</t>
+  </si>
+  <si>
+    <t>Glinski et al. 2021</t>
   </si>
 </sst>
 </file>
@@ -635,25 +635,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -663,16 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3806413E-9CE4-4194-B643-88BCE59D4128}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1058,10 +1058,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="29">
         <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1073,16 +1073,16 @@
       <c r="E3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1092,12 +1092,12 @@
       <c r="E4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="36"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="6" t="s">
         <v>58</v>
       </c>
@@ -1107,12 +1107,12 @@
       <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="4" t="s">
         <v>57</v>
       </c>
@@ -1122,12 +1122,12 @@
       <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="36"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
         <v>56</v>
       </c>
@@ -1137,12 +1137,12 @@
       <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="5" t="s">
         <v>57</v>
       </c>
@@ -1152,12 +1152,12 @@
       <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="36"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="4" t="s">
         <v>59</v>
       </c>
@@ -1167,12 +1167,12 @@
       <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="36"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="7" t="s">
         <v>60</v>
       </c>
@@ -1182,14 +1182,14 @@
       <c r="E10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="8" t="s">
         <v>62</v>
       </c>
@@ -1199,12 +1199,12 @@
       <c r="E11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="8" t="s">
         <v>63</v>
       </c>
@@ -1214,12 +1214,12 @@
       <c r="E12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="36"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="8" t="s">
         <v>57</v>
       </c>
@@ -1229,12 +1229,12 @@
       <c r="E13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="36"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="7" t="s">
         <v>61</v>
       </c>
@@ -1244,12 +1244,12 @@
       <c r="E14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="8" t="s">
         <v>57</v>
       </c>
@@ -1259,12 +1259,12 @@
       <c r="E15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="36"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="8" t="s">
         <v>64</v>
       </c>
@@ -1274,13 +1274,13 @@
       <c r="E16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="36"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="41"/>
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="11" t="s">
         <v>77</v>
       </c>
@@ -1290,16 +1290,16 @@
       <c r="E17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="41"/>
       <c r="M17" s="11"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="11" t="s">
         <v>80</v>
       </c>
@@ -1309,8 +1309,8 @@
       <c r="E18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="36"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="41"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -1319,8 +1319,8 @@
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="11" t="s">
         <v>79</v>
       </c>
@@ -1330,8 +1330,8 @@
       <c r="E19" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="36"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="41"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -1340,8 +1340,8 @@
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="11" t="s">
         <v>78</v>
       </c>
@@ -1351,8 +1351,8 @@
       <c r="E20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="36"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="41"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -1361,8 +1361,8 @@
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="8" t="s">
         <v>57</v>
       </c>
@@ -1372,8 +1372,8 @@
       <c r="E21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="36"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="41"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -1382,8 +1382,8 @@
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="11" t="s">
         <v>81</v>
       </c>
@@ -1393,8 +1393,8 @@
       <c r="E22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="36"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="41"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
@@ -1403,8 +1403,8 @@
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="8" t="s">
         <v>57</v>
       </c>
@@ -1414,8 +1414,8 @@
       <c r="E23" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="36"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="41"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
@@ -1424,8 +1424,8 @@
       <c r="N23" s="10"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="8" t="s">
         <v>65</v>
       </c>
@@ -1435,17 +1435,17 @@
       <c r="E24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="36"/>
+      <c r="G24" s="41"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="8" t="s">
         <v>66</v>
       </c>
@@ -1455,15 +1455,15 @@
       <c r="E25" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
       <c r="N25" s="10"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="8" t="s">
         <v>67</v>
       </c>
@@ -1473,12 +1473,12 @@
       <c r="E26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="8" t="s">
         <v>57</v>
       </c>
@@ -1488,12 +1488,12 @@
       <c r="E27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="41"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="8" t="s">
         <v>68</v>
       </c>
@@ -1503,12 +1503,12 @@
       <c r="E28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="8" t="s">
         <v>57</v>
       </c>
@@ -1518,12 +1518,12 @@
       <c r="E29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="8" t="s">
         <v>69</v>
       </c>
@@ -1533,12 +1533,12 @@
       <c r="E30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="8" t="s">
         <v>70</v>
       </c>
@@ -1548,16 +1548,16 @@
       <c r="E31" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="41"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="8" t="s">
         <v>76</v>
       </c>
@@ -1567,14 +1567,14 @@
       <c r="E32" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="36"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="41"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="27"/>
+      <c r="M32" s="29"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="8" t="s">
         <v>75</v>
       </c>
@@ -1584,14 +1584,14 @@
       <c r="E33" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="36"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="41"/>
       <c r="L33" s="9"/>
-      <c r="M33" s="28"/>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="8" t="s">
         <v>71</v>
       </c>
@@ -1601,16 +1601,16 @@
       <c r="E34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="36"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="41"/>
       <c r="J34" s="8"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
-      <c r="M34" s="28"/>
+      <c r="M34" s="33"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="8" t="s">
         <v>72</v>
       </c>
@@ -1620,16 +1620,16 @@
       <c r="E35" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="36"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="41"/>
       <c r="J35" s="8"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
-      <c r="M35" s="28"/>
+      <c r="M35" s="33"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
@@ -1639,16 +1639,16 @@
       <c r="E36" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="36"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="41"/>
       <c r="J36" s="7"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
-      <c r="M36" s="28"/>
+      <c r="M36" s="33"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="8" t="s">
         <v>74</v>
       </c>
@@ -1658,20 +1658,20 @@
       <c r="E37" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="29"/>
-      <c r="G37" s="36"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="41"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37" s="8"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
-      <c r="M37" s="28"/>
+      <c r="M37" s="33"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="37">
         <v>90</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -1683,10 +1683,10 @@
       <c r="E38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="42" t="s">
         <v>94</v>
       </c>
       <c r="H38"/>
@@ -1694,11 +1694,11 @@
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
-      <c r="M38" s="28"/>
+      <c r="M38" s="33"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="11" t="s">
         <v>84</v>
       </c>
@@ -1708,12 +1708,12 @@
       <c r="E39" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="29"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="37"/>
       <c r="C40" s="11" t="s">
         <v>85</v>
       </c>
@@ -1723,14 +1723,14 @@
       <c r="E40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="G40" s="29"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="11" t="s">
         <v>86</v>
       </c>
@@ -1740,12 +1740,12 @@
       <c r="E41" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="33"/>
-      <c r="G41" s="29"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="11" t="s">
         <v>87</v>
       </c>
@@ -1755,14 +1755,14 @@
       <c r="E42" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="32" t="s">
+      <c r="F42" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="G42" s="29"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="29"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="8" t="s">
         <v>57</v>
       </c>
@@ -1772,12 +1772,12 @@
       <c r="E43" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="33"/>
-      <c r="G43" s="29"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="29"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="11" t="s">
         <v>88</v>
       </c>
@@ -1787,14 +1787,14 @@
       <c r="E44" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="29"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="29"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="11" t="s">
         <v>89</v>
       </c>
@@ -1804,12 +1804,12 @@
       <c r="E45" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F45" s="33"/>
-      <c r="G45" s="29"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="29"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="11" t="s">
         <v>90</v>
       </c>
@@ -1819,14 +1819,14 @@
       <c r="E46" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="32" t="s">
+      <c r="F46" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="G46" s="29"/>
+      <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="29"/>
-      <c r="B47" s="30"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="11" t="s">
         <v>91</v>
       </c>
@@ -1836,14 +1836,14 @@
       <c r="E47" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F47" s="33"/>
-      <c r="G47" s="29"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="11" t="s">
@@ -1858,13 +1858,13 @@
       <c r="F48" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="27" t="s">
+      <c r="G48" s="29" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="11" t="s">
         <v>96</v>
       </c>
@@ -1877,12 +1877,12 @@
       <c r="F49" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G49" s="27"/>
+      <c r="G49" s="29"/>
       <c r="I49" s="16"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="11" t="s">
         <v>97</v>
       </c>
@@ -1895,11 +1895,11 @@
       <c r="F50" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G50" s="27"/>
+      <c r="G50" s="29"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="11" t="s">
         <v>98</v>
       </c>
@@ -1912,12 +1912,12 @@
       <c r="F51" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="29"/>
       <c r="I51" s="16"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="11" t="s">
         <v>99</v>
       </c>
@@ -1930,17 +1930,17 @@
       <c r="F52" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G52" s="27"/>
-    </row>
-    <row r="53" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="38" t="s">
+      <c r="G52" s="29"/>
+    </row>
+    <row r="53" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="34" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>24</v>
@@ -1951,7 +1951,7 @@
       <c r="F53" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G53" s="38" t="s">
+      <c r="G53" s="34" t="s">
         <v>25</v>
       </c>
       <c r="H53" s="23"/>
@@ -1961,11 +1961,11 @@
       <c r="L53" s="23"/>
       <c r="M53" s="23"/>
     </row>
-    <row r="54" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="42"/>
-      <c r="B54" s="42"/>
+    <row r="54" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="35"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>24</v>
@@ -1976,7 +1976,7 @@
       <c r="F54" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="42"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="23"/>
       <c r="I54" s="23"/>
       <c r="J54" s="23"/>
@@ -1984,11 +1984,11 @@
       <c r="L54" s="23"/>
       <c r="M54" s="23"/>
     </row>
-    <row r="55" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="42"/>
-      <c r="B55" s="42"/>
+    <row r="55" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>24</v>
@@ -1999,7 +1999,7 @@
       <c r="F55" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="G55" s="42"/>
+      <c r="G55" s="35"/>
       <c r="H55" s="23"/>
       <c r="I55" s="23"/>
       <c r="J55" s="23"/>
@@ -2007,11 +2007,11 @@
       <c r="L55" s="23"/>
       <c r="M55" s="23"/>
     </row>
-    <row r="56" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="42"/>
-      <c r="B56" s="42"/>
+    <row r="56" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>24</v>
@@ -2022,7 +2022,7 @@
       <c r="F56" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G56" s="42"/>
+      <c r="G56" s="35"/>
       <c r="H56" s="23"/>
       <c r="I56" s="23"/>
       <c r="J56" s="23"/>
@@ -2030,11 +2030,11 @@
       <c r="L56" s="23"/>
       <c r="M56" s="23"/>
     </row>
-    <row r="57" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="42"/>
-      <c r="B57" s="42"/>
+    <row r="57" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="35"/>
+      <c r="B57" s="35"/>
       <c r="C57" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>24</v>
@@ -2045,7 +2045,7 @@
       <c r="F57" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G57" s="42"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="23"/>
       <c r="I57" s="23"/>
       <c r="J57" s="23"/>
@@ -2054,10 +2054,10 @@
       <c r="M57" s="23"/>
     </row>
     <row r="58" spans="1:13" s="23" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
+      <c r="A58" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="37">
+      <c r="B58" s="36">
         <v>96</v>
       </c>
       <c r="C58" s="24" t="s">
@@ -2072,13 +2072,13 @@
       <c r="F58" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G58" s="37" t="s">
+      <c r="G58" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="23" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
-      <c r="B59" s="30"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="21" t="s">
         <v>106</v>
       </c>
@@ -2091,13 +2091,13 @@
       <c r="F59" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G59" s="30"/>
+      <c r="G59" s="37"/>
     </row>
     <row r="60" spans="1:13" s="23" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="37">
+      <c r="B60" s="36">
         <v>48</v>
       </c>
       <c r="C60" s="23" t="s">
@@ -2112,14 +2112,14 @@
       <c r="F60" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G60" s="37" t="s">
+      <c r="G60" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:13" s="23" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="39"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="40" t="s">
+      <c r="A61" s="38"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="27" t="s">
         <v>109</v>
       </c>
       <c r="D61" s="22" t="s">
@@ -2131,13 +2131,13 @@
       <c r="F61" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G61" s="30"/>
+      <c r="G61" s="37"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -2149,16 +2149,16 @@
       <c r="E62" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F62" s="32" t="s">
+      <c r="F62" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G62" s="27" t="s">
+      <c r="G62" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="29"/>
-      <c r="B63" s="29"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="11" t="s">
         <v>115</v>
       </c>
@@ -2168,12 +2168,12 @@
       <c r="E63" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F63" s="33"/>
-      <c r="G63" s="29"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="30"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A64" s="29"/>
-      <c r="B64" s="29"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="30"/>
       <c r="C64" s="11" t="s">
         <v>116</v>
       </c>
@@ -2183,14 +2183,14 @@
       <c r="E64" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F64" s="32" t="s">
+      <c r="F64" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="G64" s="29"/>
+      <c r="G64" s="30"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="29"/>
-      <c r="B65" s="29"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="30"/>
       <c r="C65" s="11" t="s">
         <v>117</v>
       </c>
@@ -2200,12 +2200,12 @@
       <c r="E65" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="33"/>
-      <c r="G65" s="29"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="30"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="29"/>
-      <c r="B66" s="29"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="6" t="s">
         <v>57</v>
       </c>
@@ -2215,14 +2215,14 @@
       <c r="E66" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F66" s="32" t="s">
+      <c r="F66" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="29"/>
+      <c r="G66" s="30"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="29"/>
-      <c r="B67" s="29"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="11" t="s">
         <v>118</v>
       </c>
@@ -2232,12 +2232,12 @@
       <c r="E67" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F67" s="33"/>
-      <c r="G67" s="29"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="30"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="29"/>
-      <c r="B68" s="29"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
       <c r="C68" s="11" t="s">
         <v>119</v>
       </c>
@@ -2247,14 +2247,14 @@
       <c r="E68" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F68" s="32" t="s">
+      <c r="F68" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="G68" s="29"/>
+      <c r="G68" s="30"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="29"/>
-      <c r="B69" s="29"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="11" t="s">
         <v>120</v>
       </c>
@@ -2264,12 +2264,12 @@
       <c r="E69" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F69" s="33"/>
-      <c r="G69" s="29"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="30"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="29"/>
-      <c r="B70" s="29"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="11" t="s">
         <v>121</v>
       </c>
@@ -2279,14 +2279,14 @@
       <c r="E70" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F70" s="32" t="s">
+      <c r="F70" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="G70" s="29"/>
+      <c r="G70" s="30"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="29"/>
-      <c r="B71" s="29"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="11" t="s">
         <v>122</v>
       </c>
@@ -2296,18 +2296,18 @@
       <c r="E71" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="28"/>
-      <c r="G71" s="29"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="30"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="27" t="s">
+      <c r="A72" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B72" s="27" t="s">
+      <c r="B72" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>21</v>
@@ -2318,15 +2318,15 @@
       <c r="F72" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G72" s="27" t="s">
+      <c r="G72" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="29"/>
-      <c r="B73" s="29"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D73" s="14" t="s">
         <v>21</v>
@@ -2337,13 +2337,13 @@
       <c r="F73" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G73" s="29"/>
+      <c r="G73" s="30"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="29"/>
-      <c r="B74" s="29"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="30"/>
       <c r="C74" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D74" s="14" t="s">
         <v>21</v>
@@ -2354,13 +2354,13 @@
       <c r="F74" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="29"/>
+      <c r="G74" s="30"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="27" t="s">
+      <c r="B75" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C75" s="11" t="s">
@@ -2375,13 +2375,13 @@
       <c r="F75" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G75" s="27" t="s">
+      <c r="G75" s="29" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="29"/>
-      <c r="B76" s="29"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="11" t="s">
         <v>125</v>
       </c>
@@ -2394,12 +2394,12 @@
       <c r="F76" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G76" s="29"/>
+      <c r="G76" s="30"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="29"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="40" t="s">
+      <c r="A77" s="30"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="27" t="s">
         <v>126</v>
       </c>
       <c r="D77" s="14" t="s">
@@ -2411,17 +2411,17 @@
       <c r="F77" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G77" s="29"/>
+      <c r="G77" s="30"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="27" t="s">
+      <c r="A78" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="B78" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="D78" s="14" t="s">
         <v>40</v>
@@ -2432,15 +2432,15 @@
       <c r="F78" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G78" s="27" t="s">
+      <c r="G78" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="29"/>
-      <c r="B79" s="29"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D79" s="14" t="s">
         <v>40</v>
@@ -2451,13 +2451,13 @@
       <c r="F79" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="G79" s="29"/>
+      <c r="G79" s="30"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="29"/>
-      <c r="B80" s="29"/>
-      <c r="C80" s="40" t="s">
-        <v>130</v>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="D80" s="14" t="s">
         <v>40</v>
@@ -2468,7 +2468,7 @@
       <c r="F80" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G80" s="29"/>
+      <c r="G80" s="30"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="19"/>
@@ -2511,6 +2511,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="M32:M38"/>
+    <mergeCell ref="F17:F23"/>
+    <mergeCell ref="F10:F16"/>
+    <mergeCell ref="B3:B37"/>
+    <mergeCell ref="F3:F9"/>
+    <mergeCell ref="B38:B47"/>
+    <mergeCell ref="G38:G47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G48:G52"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="A3:A37"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="G3:G37"/>
+    <mergeCell ref="A38:A47"/>
+    <mergeCell ref="A62:A71"/>
+    <mergeCell ref="G53:G57"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="G60:G61"/>
     <mergeCell ref="G78:G80"/>
     <mergeCell ref="A78:A80"/>
     <mergeCell ref="B78:B80"/>
@@ -2527,36 +2557,6 @@
     <mergeCell ref="B75:B77"/>
     <mergeCell ref="G62:G71"/>
     <mergeCell ref="B62:B71"/>
-    <mergeCell ref="A62:A71"/>
-    <mergeCell ref="G53:G57"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G48:G52"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="A3:A37"/>
-    <mergeCell ref="F24:F30"/>
-    <mergeCell ref="F31:F37"/>
-    <mergeCell ref="G3:G37"/>
-    <mergeCell ref="A38:A47"/>
-    <mergeCell ref="M32:M38"/>
-    <mergeCell ref="F17:F23"/>
-    <mergeCell ref="F10:F16"/>
-    <mergeCell ref="B3:B37"/>
-    <mergeCell ref="F3:F9"/>
-    <mergeCell ref="B38:B47"/>
-    <mergeCell ref="G38:G47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>